<commit_message>
PIK3CA SST gene functions
</commit_message>
<xml_diff>
--- a/SST_Data_function table.xlsx
+++ b/SST_Data_function table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salome\Documents\4.FS\Bioinfo\GitHub\project-01-group-04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisa-\Desktop\Studium\4. FS\Bioinfo\project-01-group-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1782C0BE-5C44-4F6B-845E-072EB05B54A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4EF87-9C61-4EFB-836E-791E29A0DFD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5410" yWindow="2390" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{14626772-5318-4F08-8B22-3A6AEDECE32E}"/>
+    <workbookView xWindow="-5028" yWindow="6876" windowWidth="12960" windowHeight="8964" activeTab="3" xr2:uid="{14626772-5318-4F08-8B22-3A6AEDECE32E}"/>
   </bookViews>
   <sheets>
     <sheet name="ERBB2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="225">
   <si>
     <t>BCL9L</t>
   </si>
@@ -601,6 +601,114 @@
   </si>
   <si>
     <t>Tensin-3; cell migration and actin remodeling; mammary cell migration</t>
+  </si>
+  <si>
+    <t>Adenomatous polyposis coli protein: tumour suppressor acting as a promotor of Wnt signalling and regulator of cell migration</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/P25054</t>
+  </si>
+  <si>
+    <t>Sodium/potassium-transporting ATPase subunit beta-3: catalysis of ATP hydrolysis</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/P54709</t>
+  </si>
+  <si>
+    <t>Bromodomain-containing protein 2: role in spermatogenesis and folliculogenesis with regulatory effect in chromatin remodelling and nucleosome assembly, transcription regulator of CCND1</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/P25440</t>
+  </si>
+  <si>
+    <t>Cytoplasmic FMR1-interacting protein 1: ediator of translational represseion, role in epithelial morphogenesis by regulation of actin remodelling and axon outgrowth (maybe tumour invasion suppresor)</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q7L576</t>
+  </si>
+  <si>
+    <t>Probable dimethyladenosine transferase: involved in RNA editing and processing of rRNA</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q9UNQ2</t>
+  </si>
+  <si>
+    <t>GA-binding protein alpha chain: transcription factor in cell differentiation</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q06546</t>
+  </si>
+  <si>
+    <t>Cyclin-G-associated kinase: acts as an auxilin homolog uncoating clathrin vesicles, expression peaks at G1 phase</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/O14976</t>
+  </si>
+  <si>
+    <t>G-protein coupled receptor 61: contitutive activation aof G(s) signalling pathway, may be involved in regulation of food intake and body weight</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q9BZJ8</t>
+  </si>
+  <si>
+    <t>Orexin receptor type 1: excitatory receptor regulating ERK1 and ERK2 cascade and cytosolic Calcium concentration</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/O43613</t>
+  </si>
+  <si>
+    <t>Histone H2B type 1-C/E/F/G/I: core component of nucleosomes</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/P62807</t>
+  </si>
+  <si>
+    <t>Protein max: trancription regulator eventually ivolved in chromati remodelling, repressor of MYC</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/P61244</t>
+  </si>
+  <si>
+    <t>Non-structural maintenance of chromosomes element 4 homolog A: part of a complex involved in homologous recombination of sister chromatids and telomere maintenance, role in response to DNA damage</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q9NXX6</t>
+  </si>
+  <si>
+    <t>DNA polymerase theta: promotes microhomology-mediated end-joining in response to double-strand breaks</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/O75417</t>
+  </si>
+  <si>
+    <t>Protein prenyltransferase alpha subunit repeat-containing protein 1</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q7Z6K3</t>
+  </si>
+  <si>
+    <t>Replication factor C subunit 1: promotes elongation of primed DNA tmeplates, eventually role in DNA replacation and/or repair</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/P35251</t>
+  </si>
+  <si>
+    <t>Sorting and assembly machinery component 50 homolog: role in maintenance of struture of mitochondria (especially respiratory chain complexes)</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q9Y512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4F2 cell-surface antigen heavy chain: component of aminp acid transporter complexes </t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/P08195-1</t>
+  </si>
+  <si>
+    <t>tRNA methyltransferase 10 homolog C: involved in mitchondrial tRNA maturation</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q7L0Y3</t>
   </si>
 </sst>
 </file>
@@ -679,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -696,6 +804,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1013,18 +1124,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D4647E-F838-463E-B1EA-207682381C91}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.81640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.77734375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
@@ -1038,7 +1149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1166,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1072,7 +1183,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1089,7 +1200,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1106,7 +1217,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1123,7 +1234,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1140,7 +1251,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1157,7 +1268,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1285,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1191,7 +1302,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1319,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1225,7 +1336,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1242,7 +1353,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1259,7 +1370,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1276,7 +1387,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1293,7 +1404,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1310,7 +1421,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1341,14 +1452,14 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="42.81640625" customWidth="1"/>
-    <col min="4" max="4" width="38.90625" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
@@ -1362,7 +1473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -1379,7 +1490,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1396,7 +1507,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1413,7 +1524,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1430,7 +1541,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -1447,7 +1558,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1464,7 +1575,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -1481,7 +1592,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="59.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1498,7 +1609,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -1515,7 +1626,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -1532,7 +1643,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1549,7 +1660,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1566,7 +1677,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1583,7 +1694,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -1600,7 +1711,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1617,14 +1728,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E19" s="6"/>
     </row>
   </sheetData>
@@ -1637,18 +1748,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DF335A-5F5C-48C6-B07A-905A289F6DB7}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="42.81640625" customWidth="1"/>
-    <col min="4" max="4" width="38.90625" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>70</v>
       </c>
@@ -1662,7 +1773,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -1679,7 +1790,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -1696,7 +1807,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1713,7 +1824,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -1730,7 +1841,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
@@ -1747,7 +1858,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -1764,7 +1875,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
@@ -1781,7 +1892,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
@@ -1798,7 +1909,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
@@ -1815,7 +1926,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1832,7 +1943,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
@@ -1849,7 +1960,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1866,7 +1977,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="49.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
@@ -1883,7 +1994,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -1900,7 +2011,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>67</v>
       </c>
@@ -1917,7 +2028,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -1934,7 +2045,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1960,32 +2071,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA6A8EF-2F16-4AAA-844D-A58EBF649AB6}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="42.81640625" customWidth="1"/>
-    <col min="4" max="4" width="38.90625" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="28" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
@@ -1995,8 +2106,14 @@
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -2006,8 +2123,14 @@
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
@@ -2017,8 +2140,14 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -2028,8 +2157,14 @@
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>75</v>
       </c>
@@ -2039,8 +2174,14 @@
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D6" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -2050,8 +2191,14 @@
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -2061,8 +2208,14 @@
       <c r="C8" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>79</v>
       </c>
@@ -2072,8 +2225,14 @@
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D9" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>80</v>
       </c>
@@ -2083,8 +2242,14 @@
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D10" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>81</v>
       </c>
@@ -2094,8 +2259,14 @@
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D11" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -2105,8 +2276,14 @@
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D12" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>83</v>
       </c>
@@ -2116,8 +2293,14 @@
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D13" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>84</v>
       </c>
@@ -2127,8 +2310,14 @@
       <c r="C14" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D14" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -2138,8 +2327,14 @@
       <c r="C15" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D15" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>87</v>
       </c>
@@ -2149,8 +2344,14 @@
       <c r="C16" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D16" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
@@ -2160,8 +2361,14 @@
       <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D17" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>90</v>
       </c>
@@ -2171,8 +2378,14 @@
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D18" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>91</v>
       </c>
@@ -2182,8 +2395,15 @@
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D19" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>224</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>